<commit_message>
Minor pas2716 test updates
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/R45VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/R45VIN_UT_SS.xlsx
@@ -191,10 +191,10 @@
     <t>Gt_R45</t>
   </si>
   <si>
-    <t>1FDEU15H&amp;K</t>
-  </si>
-  <si>
-    <t>SYMBOL_2000_SS_TEST</t>
+    <t>BBBKN3DD&amp;E</t>
+  </si>
+  <si>
+    <t>SYMBOL_200</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>